<commit_message>
add missing trunc for div in excel.
</commit_message>
<xml_diff>
--- a/2021day24/alu2021day24.xlsx
+++ b/2021day24/alu2021day24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feri\git\AdventOfCode\2021day24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E513C41-C81B-486C-9653-1146C26C46CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CDC3C7-45C7-42F3-AF90-6D2EB3E42E8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{56EE513B-A1A9-4F6D-A498-8BB4479BB114}"/>
   </bookViews>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7033259C-CD9B-4E2A-BEA6-C711622595CA}">
   <dimension ref="B4:AI271"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD269" sqref="AD269"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z257" sqref="Z257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <f>Z9/AD10</f>
+        <f>TRUNC(Z9/AD10,0)</f>
         <v>0</v>
       </c>
       <c r="AB10" s="4" t="s">
@@ -1193,7 +1193,7 @@
         <v>21</v>
       </c>
       <c r="Z29">
-        <f>Z28/AD29</f>
+        <f>TRUNC(Z28/AD29,0)</f>
         <v>21</v>
       </c>
       <c r="AB29" s="4" t="s">
@@ -1683,7 +1683,7 @@
         <v>17</v>
       </c>
       <c r="Z48">
-        <f>Z47/AD48</f>
+        <f>TRUNC(Z47/AD48,0)</f>
         <v>563</v>
       </c>
       <c r="AB48" s="4" t="s">
@@ -2263,7 +2263,7 @@
         <v>9</v>
       </c>
       <c r="Z67">
-        <f>Z66/AD67</f>
+        <f>TRUNC(Z66/AD67,0)</f>
         <v>14647</v>
       </c>
       <c r="AB67" t="s">
@@ -2843,8 +2843,8 @@
         <v>6</v>
       </c>
       <c r="Z86">
-        <f>Z85/AD86</f>
-        <v>14647.23076923077</v>
+        <f>TRUNC(Z85/AD86,0)</f>
+        <v>14647</v>
       </c>
       <c r="AB86" s="6" t="s">
         <v>27</v>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="Z87">
         <f t="shared" ref="Z87:Z93" si="34">Z86</f>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB87" t="s">
         <v>28</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="Z88">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB88" t="s">
         <v>10</v>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="Z89">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB89" t="s">
         <v>11</v>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="Z90">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB90" t="s">
         <v>12</v>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="Z91">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB91" t="s">
         <v>13</v>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="Z92">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB92" t="s">
         <v>14</v>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="Z93">
         <f t="shared" si="34"/>
-        <v>14647.23076923077</v>
+        <v>14647</v>
       </c>
       <c r="AB93" t="s">
         <v>15</v>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="Z94">
         <f>Z93*Y93</f>
-        <v>380828</v>
+        <v>380822</v>
       </c>
       <c r="AB94" t="s">
         <v>16</v>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="Z95">
         <f t="shared" ref="Z95:Z98" si="38">Z94</f>
-        <v>380828</v>
+        <v>380822</v>
       </c>
       <c r="AB95" t="s">
         <v>12</v>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="Z96">
         <f t="shared" si="38"/>
-        <v>380828</v>
+        <v>380822</v>
       </c>
       <c r="AB96" t="s">
         <v>17</v>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="Z97">
         <f t="shared" si="38"/>
-        <v>380828</v>
+        <v>380822</v>
       </c>
       <c r="AB97" t="s">
         <v>26</v>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="Z98">
         <f t="shared" si="38"/>
-        <v>380828</v>
+        <v>380822</v>
       </c>
       <c r="AB98" t="s">
         <v>14</v>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="Z99">
         <f>Z98+Y98</f>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB99" t="s">
         <v>19</v>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="Z100" s="3">
         <f t="shared" ref="Z100:Z104" si="41">Z99</f>
-        <v>380834</v>
+        <v>380828</v>
       </c>
     </row>
     <row r="101" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="Z101">
         <f t="shared" si="41"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB101" t="s">
         <v>4</v>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="Z102">
         <f t="shared" si="41"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB102" t="s">
         <v>5</v>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="X103">
         <f>X102+Z102</f>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="Y103">
         <f t="shared" si="40"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="Z103">
         <f t="shared" si="41"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB103" t="s">
         <v>6</v>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="X104">
         <f>MOD(X103,26)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Y104">
         <f t="shared" si="40"/>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="Z104">
         <f t="shared" si="41"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB104" t="s">
         <v>7</v>
@@ -3416,15 +3416,15 @@
       </c>
       <c r="X105">
         <f t="shared" ref="X105" si="43">X104</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Y105">
         <f t="shared" si="40"/>
         <v>6</v>
       </c>
       <c r="Z105">
-        <f>Z104/AD105</f>
-        <v>380834</v>
+        <f>TRUNC(Z104/AD105,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB105" t="s">
         <v>8</v>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="X106">
         <f>X105+AD106</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="Y106">
         <f t="shared" si="40"/>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="Z106">
         <f t="shared" ref="Z106:Z112" si="44">Z105</f>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB106" t="s">
         <v>29</v>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="Z107">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB107" t="s">
         <v>10</v>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="Z108">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB108" t="s">
         <v>11</v>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="Z109">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB109" t="s">
         <v>12</v>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="Z110">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB110" t="s">
         <v>13</v>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="Z111">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB111" t="s">
         <v>14</v>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="Z112">
         <f t="shared" si="44"/>
-        <v>380834</v>
+        <v>380828</v>
       </c>
       <c r="AB112" t="s">
         <v>15</v>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="Z113">
         <f>Z112*Y112</f>
-        <v>9901684</v>
+        <v>9901528</v>
       </c>
       <c r="AB113" t="s">
         <v>16</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="Z114">
         <f t="shared" ref="Z114:Z117" si="48">Z113</f>
-        <v>9901684</v>
+        <v>9901528</v>
       </c>
       <c r="AB114" t="s">
         <v>12</v>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="Z115">
         <f t="shared" si="48"/>
-        <v>9901684</v>
+        <v>9901528</v>
       </c>
       <c r="AB115" t="s">
         <v>17</v>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="Z116">
         <f t="shared" si="48"/>
-        <v>9901684</v>
+        <v>9901528</v>
       </c>
       <c r="AB116" t="s">
         <v>15</v>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="Z117">
         <f t="shared" si="48"/>
-        <v>9901684</v>
+        <v>9901528</v>
       </c>
       <c r="AB117" t="s">
         <v>14</v>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="Z118">
         <f>Z117+Y117</f>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="AB118" t="s">
         <v>19</v>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="Z119" s="3">
         <f t="shared" ref="Z119:Z123" si="51">Z118</f>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
     </row>
     <row r="120" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="Z120">
         <f t="shared" si="51"/>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="AB120" t="s">
         <v>4</v>
@@ -3911,7 +3911,7 @@
       </c>
       <c r="Z121">
         <f t="shared" si="51"/>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="AB121" t="s">
         <v>5</v>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="X122">
         <f>X121+Z121</f>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="Y122">
         <f t="shared" si="50"/>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="Z122">
         <f t="shared" si="51"/>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="AB122" t="s">
         <v>6</v>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="Z123">
         <f t="shared" si="51"/>
-        <v>9901687</v>
+        <v>9901531</v>
       </c>
       <c r="AB123" t="s">
         <v>7</v>
@@ -4003,8 +4003,8 @@
         <v>3</v>
       </c>
       <c r="Z124">
-        <f>Z123/AD124</f>
-        <v>380834.11538461538</v>
+        <f>TRUNC(Z123/AD124,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB124" s="6" t="s">
         <v>27</v>
@@ -4038,7 +4038,7 @@
       </c>
       <c r="Z125">
         <f t="shared" ref="Z125:Z131" si="54">Z124</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB125" t="s">
         <v>30</v>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="Z126">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB126" t="s">
         <v>10</v>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="Z127">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB127" t="s">
         <v>11</v>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="Z128">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB128" t="s">
         <v>12</v>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="Z129">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB129" t="s">
         <v>13</v>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="Z130">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB130" t="s">
         <v>14</v>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="Z131">
         <f t="shared" si="54"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB131" t="s">
         <v>15</v>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="Z132">
         <f>Z131*Y131</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB132" t="s">
         <v>16</v>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="Z133">
         <f t="shared" ref="Z133:Z136" si="58">Z132</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB133" t="s">
         <v>12</v>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="Z134">
         <f t="shared" si="58"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB134" t="s">
         <v>17</v>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="Z135">
         <f t="shared" si="58"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB135" t="s">
         <v>31</v>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="Z136">
         <f t="shared" si="58"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB136" t="s">
         <v>14</v>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="Z137">
         <f>Z136+Y136</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB137" t="s">
         <v>19</v>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="Z138" s="3">
         <f t="shared" ref="Z138:Z142" si="61">Z137</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
     </row>
     <row r="139" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4460,7 +4460,7 @@
       </c>
       <c r="Z139">
         <f t="shared" si="61"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB139" t="s">
         <v>4</v>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="Z140">
         <f t="shared" si="61"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB140" t="s">
         <v>5</v>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="X141">
         <f>X140+Z140</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="Y141">
         <f t="shared" si="60"/>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="Z141">
         <f t="shared" si="61"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB141" t="s">
         <v>6</v>
@@ -4545,7 +4545,7 @@
       </c>
       <c r="X142">
         <f>MOD(X141,26)</f>
-        <v>12.11538461537566</v>
+        <v>6</v>
       </c>
       <c r="Y142">
         <f t="shared" si="60"/>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="Z142">
         <f t="shared" si="61"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB142" t="s">
         <v>7</v>
@@ -4576,15 +4576,15 @@
       </c>
       <c r="X143">
         <f t="shared" ref="X143" si="63">X142</f>
-        <v>12.11538461537566</v>
+        <v>6</v>
       </c>
       <c r="Y143">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="Z143">
-        <f>Z142/AD143</f>
-        <v>380834.11538461538</v>
+        <f>TRUNC(Z142/AD143,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB143" t="s">
         <v>8</v>
@@ -4610,7 +4610,7 @@
       </c>
       <c r="X144">
         <f>X143+AD144</f>
-        <v>22.11538461537566</v>
+        <v>16</v>
       </c>
       <c r="Y144">
         <f t="shared" si="60"/>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="Z144">
         <f t="shared" ref="Z144:Z150" si="64">Z143</f>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB144" t="s">
         <v>32</v>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="Z145">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB145" t="s">
         <v>10</v>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="Z146">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB146" t="s">
         <v>11</v>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="Z147">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB147" t="s">
         <v>12</v>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="Z148">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB148" t="s">
         <v>13</v>
@@ -4772,7 +4772,7 @@
       </c>
       <c r="Z149">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB149" t="s">
         <v>14</v>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="Z150">
         <f t="shared" si="64"/>
-        <v>380834.11538461538</v>
+        <v>380828</v>
       </c>
       <c r="AB150" t="s">
         <v>15</v>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="Z151">
         <f>Z150*Y150</f>
-        <v>9901687</v>
+        <v>9901528</v>
       </c>
       <c r="AB151" t="s">
         <v>16</v>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="Z152">
         <f t="shared" ref="Z152:Z155" si="68">Z151</f>
-        <v>9901687</v>
+        <v>9901528</v>
       </c>
       <c r="AB152" t="s">
         <v>12</v>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="Z153">
         <f t="shared" si="68"/>
-        <v>9901687</v>
+        <v>9901528</v>
       </c>
       <c r="AB153" t="s">
         <v>17</v>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="Z154">
         <f t="shared" si="68"/>
-        <v>9901687</v>
+        <v>9901528</v>
       </c>
       <c r="AB154" t="s">
         <v>22</v>
@@ -4957,7 +4957,7 @@
       </c>
       <c r="Z155">
         <f t="shared" si="68"/>
-        <v>9901687</v>
+        <v>9901528</v>
       </c>
       <c r="AB155" t="s">
         <v>14</v>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="Z156">
         <f>Z155+Y155</f>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="AB156" t="s">
         <v>19</v>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="Z157" s="3">
         <f t="shared" ref="Z157:Z161" si="71">Z156</f>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
     </row>
     <row r="158" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="Z158">
         <f t="shared" si="71"/>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="AB158" t="s">
         <v>4</v>
@@ -5071,7 +5071,7 @@
       </c>
       <c r="Z159">
         <f t="shared" si="71"/>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="AB159" t="s">
         <v>5</v>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="X160">
         <f>X159+Z159</f>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="Y160">
         <f t="shared" si="70"/>
@@ -5102,7 +5102,7 @@
       </c>
       <c r="Z160">
         <f t="shared" si="71"/>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="AB160" t="s">
         <v>6</v>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="X161">
         <f>MOD(X160,26)</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Y161">
         <f t="shared" si="70"/>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="Z161">
         <f t="shared" si="71"/>
-        <v>9901697</v>
+        <v>9901538</v>
       </c>
       <c r="AB161" t="s">
         <v>7</v>
@@ -5156,15 +5156,15 @@
       </c>
       <c r="X162">
         <f t="shared" ref="X162" si="73">X161</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Y162">
         <f t="shared" si="70"/>
         <v>10</v>
       </c>
       <c r="Z162">
-        <f>Z161/AD162</f>
-        <v>380834.5</v>
+        <f>TRUNC(Z161/AD162,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB162" s="6" t="s">
         <v>27</v>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="X163">
         <f>X162+AD163</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Y163">
         <f t="shared" si="70"/>
@@ -5198,7 +5198,7 @@
       </c>
       <c r="Z163">
         <f t="shared" ref="Z163:Z169" si="74">Z162</f>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB163" t="s">
         <v>33</v>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="Z164">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB164" t="s">
         <v>10</v>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="Z165">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB165" t="s">
         <v>11</v>
@@ -5290,7 +5290,7 @@
       </c>
       <c r="Z166">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB166" t="s">
         <v>12</v>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="Z167">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB167" t="s">
         <v>13</v>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="Z168">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB168" t="s">
         <v>14</v>
@@ -5383,7 +5383,7 @@
       </c>
       <c r="Z169">
         <f t="shared" si="74"/>
-        <v>380834.5</v>
+        <v>380828</v>
       </c>
       <c r="AB169" t="s">
         <v>15</v>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="Z170">
         <f>Z169*Y169</f>
-        <v>9901697</v>
+        <v>9901528</v>
       </c>
       <c r="AB170" t="s">
         <v>16</v>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="Z171">
         <f t="shared" ref="Z171:Z174" si="78">Z170</f>
-        <v>9901697</v>
+        <v>9901528</v>
       </c>
       <c r="AB171" t="s">
         <v>12</v>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="Z172">
         <f t="shared" si="78"/>
-        <v>9901697</v>
+        <v>9901528</v>
       </c>
       <c r="AB172" t="s">
         <v>17</v>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="Z173">
         <f t="shared" si="78"/>
-        <v>9901697</v>
+        <v>9901528</v>
       </c>
       <c r="AB173" t="s">
         <v>18</v>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="Z174">
         <f t="shared" si="78"/>
-        <v>9901697</v>
+        <v>9901528</v>
       </c>
       <c r="AB174" t="s">
         <v>14</v>
@@ -5568,7 +5568,7 @@
       </c>
       <c r="Z175">
         <f>Z174+Y174</f>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="AB175" t="s">
         <v>19</v>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="Z176" s="3">
         <f t="shared" ref="Z176:Z180" si="81">Z175</f>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
     </row>
     <row r="177" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="Z177">
         <f t="shared" si="81"/>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="AB177" t="s">
         <v>4</v>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="Z178">
         <f t="shared" si="81"/>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="AB178" t="s">
         <v>5</v>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="X179">
         <f>X178+Z178</f>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="Y179">
         <f t="shared" si="80"/>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="Z179">
         <f t="shared" si="81"/>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="AB179" t="s">
         <v>6</v>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="X180">
         <f>MOD(X179,26)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Y180">
         <f t="shared" si="80"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="Z180">
         <f t="shared" si="81"/>
-        <v>9901711</v>
+        <v>9901542</v>
       </c>
       <c r="AB180" t="s">
         <v>7</v>
@@ -5736,15 +5736,15 @@
       </c>
       <c r="X181">
         <f t="shared" ref="X181" si="83">X180</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Y181">
         <f t="shared" si="80"/>
         <v>14</v>
       </c>
       <c r="Z181">
-        <f>Z180/AD181</f>
-        <v>380835.03846153844</v>
+        <f>TRUNC(Z180/AD181,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB181" s="6" t="s">
         <v>27</v>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="X182">
         <f>X181+AD182</f>
-        <v>-3</v>
+        <v>10</v>
       </c>
       <c r="Y182">
         <f t="shared" si="80"/>
@@ -5778,7 +5778,7 @@
       </c>
       <c r="Z182">
         <f t="shared" ref="Z182:Z188" si="84">Z181</f>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB182" t="s">
         <v>34</v>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="Z183">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB183" t="s">
         <v>10</v>
@@ -5839,7 +5839,7 @@
       </c>
       <c r="Z184">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB184" t="s">
         <v>11</v>
@@ -5870,7 +5870,7 @@
       </c>
       <c r="Z185">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB185" t="s">
         <v>12</v>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="Z186">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB186" t="s">
         <v>13</v>
@@ -5932,7 +5932,7 @@
       </c>
       <c r="Z187">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB187" t="s">
         <v>14</v>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="Z188">
         <f t="shared" si="84"/>
-        <v>380835.03846153844</v>
+        <v>380828</v>
       </c>
       <c r="AB188" t="s">
         <v>15</v>
@@ -5994,7 +5994,7 @@
       </c>
       <c r="Z189">
         <f>Z188*Y188</f>
-        <v>9901711</v>
+        <v>9901528</v>
       </c>
       <c r="AB189" t="s">
         <v>16</v>
@@ -6025,7 +6025,7 @@
       </c>
       <c r="Z190">
         <f t="shared" ref="Z190:Z193" si="88">Z189</f>
-        <v>9901711</v>
+        <v>9901528</v>
       </c>
       <c r="AB190" t="s">
         <v>12</v>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="Z191">
         <f t="shared" si="88"/>
-        <v>9901711</v>
+        <v>9901528</v>
       </c>
       <c r="AB191" t="s">
         <v>17</v>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="Z192">
         <f t="shared" si="88"/>
-        <v>9901711</v>
+        <v>9901528</v>
       </c>
       <c r="AB192" t="s">
         <v>31</v>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="Z193">
         <f t="shared" si="88"/>
-        <v>9901711</v>
+        <v>9901528</v>
       </c>
       <c r="AB193" t="s">
         <v>14</v>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="Z194">
         <f>Z193+Y193</f>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="AB194" t="s">
         <v>19</v>
@@ -6179,7 +6179,7 @@
       </c>
       <c r="Z195" s="3">
         <f t="shared" ref="Z195:Z199" si="91">Z194</f>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
     </row>
     <row r="196" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6200,7 +6200,7 @@
       </c>
       <c r="Z196">
         <f t="shared" si="91"/>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="AB196" t="s">
         <v>4</v>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="Z197">
         <f t="shared" si="91"/>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="AB197" t="s">
         <v>5</v>
@@ -6254,7 +6254,7 @@
       </c>
       <c r="X198">
         <f>X197+Z197</f>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="Y198">
         <f t="shared" si="90"/>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="Z198">
         <f t="shared" si="91"/>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="AB198" t="s">
         <v>6</v>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="X199">
         <f>MOD(X198,26)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y199">
         <f t="shared" si="90"/>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="Z199">
         <f t="shared" si="91"/>
-        <v>9901723</v>
+        <v>9901540</v>
       </c>
       <c r="AB199" t="s">
         <v>7</v>
@@ -6316,15 +6316,15 @@
       </c>
       <c r="X200">
         <f t="shared" ref="X200" si="93">X199</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y200">
         <f t="shared" si="90"/>
         <v>12</v>
       </c>
       <c r="Z200">
-        <f>Z199/AD200</f>
-        <v>380835.5</v>
+        <f>TRUNC(Z199/AD200,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB200" s="6" t="s">
         <v>27</v>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="X201">
         <f>X200+AD201</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y201">
         <f t="shared" si="90"/>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="Z201">
         <f t="shared" ref="Z201:Z207" si="94">Z200</f>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB201" t="s">
         <v>35</v>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="Z202">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB202" t="s">
         <v>10</v>
@@ -6419,7 +6419,7 @@
       </c>
       <c r="Z203">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB203" t="s">
         <v>11</v>
@@ -6450,7 +6450,7 @@
       </c>
       <c r="Z204">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB204" t="s">
         <v>12</v>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="Z205">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB205" t="s">
         <v>13</v>
@@ -6512,7 +6512,7 @@
       </c>
       <c r="Z206">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB206" t="s">
         <v>14</v>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="Z207">
         <f t="shared" si="94"/>
-        <v>380835.5</v>
+        <v>380828</v>
       </c>
       <c r="AB207" t="s">
         <v>15</v>
@@ -6574,7 +6574,7 @@
       </c>
       <c r="Z208">
         <f>Z207*Y207</f>
-        <v>9901723</v>
+        <v>9901528</v>
       </c>
       <c r="AB208" t="s">
         <v>16</v>
@@ -6605,7 +6605,7 @@
       </c>
       <c r="Z209">
         <f t="shared" ref="Z209:Z212" si="98">Z208</f>
-        <v>9901723</v>
+        <v>9901528</v>
       </c>
       <c r="AB209" t="s">
         <v>12</v>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="Z210">
         <f t="shared" si="98"/>
-        <v>9901723</v>
+        <v>9901528</v>
       </c>
       <c r="AB210" t="s">
         <v>17</v>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="Z211">
         <f t="shared" si="98"/>
-        <v>9901723</v>
+        <v>9901528</v>
       </c>
       <c r="AB211" t="s">
         <v>36</v>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="Z212">
         <f t="shared" si="98"/>
-        <v>9901723</v>
+        <v>9901528</v>
       </c>
       <c r="AB212" t="s">
         <v>14</v>
@@ -6728,7 +6728,7 @@
       </c>
       <c r="Z213">
         <f>Z212+Y212</f>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="AB213" t="s">
         <v>19</v>
@@ -6759,7 +6759,7 @@
       </c>
       <c r="Z214" s="3">
         <f t="shared" ref="Z214:Z218" si="101">Z213</f>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
     </row>
     <row r="215" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="Z215">
         <f t="shared" si="101"/>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="AB215" t="s">
         <v>4</v>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="Z216">
         <f t="shared" si="101"/>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="AB216" t="s">
         <v>5</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="X217">
         <f>X216+Z216</f>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="Y217">
         <f t="shared" si="100"/>
@@ -6842,7 +6842,7 @@
       </c>
       <c r="Z217">
         <f t="shared" si="101"/>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="AB217" t="s">
         <v>6</v>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="X218">
         <f>MOD(X217,26)</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Y218">
         <f t="shared" si="100"/>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="Z218">
         <f t="shared" si="101"/>
-        <v>9901740</v>
+        <v>9901545</v>
       </c>
       <c r="AB218" t="s">
         <v>7</v>
@@ -6896,15 +6896,15 @@
       </c>
       <c r="X219">
         <f t="shared" ref="X219" si="103">X218</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Y219">
         <f t="shared" si="100"/>
         <v>17</v>
       </c>
       <c r="Z219">
-        <f>Z218/AD219</f>
-        <v>380836.15384615387</v>
+        <f>TRUNC(Z218/AD219,0)</f>
+        <v>380828</v>
       </c>
       <c r="AB219" s="6" t="s">
         <v>27</v>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="X220">
         <f>X219+AD220</f>
-        <v>-4</v>
+        <v>9</v>
       </c>
       <c r="Y220">
         <f t="shared" si="100"/>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="Z220">
         <f t="shared" ref="Z220:Z226" si="104">Z219</f>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB220" t="s">
         <v>37</v>
@@ -6968,7 +6968,7 @@
       </c>
       <c r="Z221">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB221" t="s">
         <v>10</v>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="Z222">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB222" t="s">
         <v>11</v>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="Z223">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB223" t="s">
         <v>12</v>
@@ -7061,7 +7061,7 @@
       </c>
       <c r="Z224">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB224" t="s">
         <v>13</v>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="Z225">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB225" t="s">
         <v>14</v>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="Z226">
         <f t="shared" si="104"/>
-        <v>380836.15384615387</v>
+        <v>380828</v>
       </c>
       <c r="AB226" t="s">
         <v>15</v>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="Z227">
         <f>Z226*Y226</f>
-        <v>9901740</v>
+        <v>9901528</v>
       </c>
       <c r="AB227" t="s">
         <v>16</v>
@@ -7185,7 +7185,7 @@
       </c>
       <c r="Z228">
         <f t="shared" ref="Z228:Z231" si="108">Z227</f>
-        <v>9901740</v>
+        <v>9901528</v>
       </c>
       <c r="AB228" t="s">
         <v>12</v>
@@ -7216,7 +7216,7 @@
       </c>
       <c r="Z229">
         <f t="shared" si="108"/>
-        <v>9901740</v>
+        <v>9901528</v>
       </c>
       <c r="AB229" t="s">
         <v>17</v>
@@ -7247,7 +7247,7 @@
       </c>
       <c r="Z230">
         <f t="shared" si="108"/>
-        <v>9901740</v>
+        <v>9901528</v>
       </c>
       <c r="AB230" t="s">
         <v>26</v>
@@ -7277,7 +7277,7 @@
       </c>
       <c r="Z231">
         <f t="shared" si="108"/>
-        <v>9901740</v>
+        <v>9901528</v>
       </c>
       <c r="AB231" t="s">
         <v>14</v>
@@ -7308,7 +7308,7 @@
       </c>
       <c r="Z232">
         <f>Z231+Y231</f>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB232" t="s">
         <v>19</v>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="Z233" s="3">
         <f t="shared" ref="Z233:Z237" si="111">Z232</f>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
     </row>
     <row r="234" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7360,7 +7360,7 @@
       </c>
       <c r="Z234">
         <f t="shared" si="111"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB234" t="s">
         <v>4</v>
@@ -7391,7 +7391,7 @@
       </c>
       <c r="Z235">
         <f t="shared" si="111"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB235" t="s">
         <v>5</v>
@@ -7414,7 +7414,7 @@
       </c>
       <c r="X236">
         <f>X235+Z235</f>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="Y236">
         <f t="shared" si="110"/>
@@ -7422,7 +7422,7 @@
       </c>
       <c r="Z236">
         <f t="shared" si="111"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB236" t="s">
         <v>6</v>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="X237">
         <f>MOD(X236,26)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Y237">
         <f t="shared" si="110"/>
@@ -7453,7 +7453,7 @@
       </c>
       <c r="Z237">
         <f t="shared" si="111"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB237" t="s">
         <v>7</v>
@@ -7476,15 +7476,15 @@
       </c>
       <c r="X238">
         <f t="shared" ref="X238" si="113">X237</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Y238">
         <f t="shared" si="110"/>
         <v>6</v>
       </c>
       <c r="Z238">
-        <f>Z237/AD238</f>
-        <v>9901746</v>
+        <f>TRUNC(Z237/AD238,0)</f>
+        <v>9901534</v>
       </c>
       <c r="AB238" t="s">
         <v>8</v>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="X239">
         <f>X238+AD239</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="Y239">
         <f t="shared" si="110"/>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="Z239">
         <f t="shared" ref="Z239:Z245" si="114">Z238</f>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB239" t="s">
         <v>38</v>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="Z240">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB240" t="s">
         <v>10</v>
@@ -7579,7 +7579,7 @@
       </c>
       <c r="Z241">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB241" t="s">
         <v>11</v>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="Z242">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB242" t="s">
         <v>12</v>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="Z243">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB243" t="s">
         <v>13</v>
@@ -7672,7 +7672,7 @@
       </c>
       <c r="Z244">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB244" t="s">
         <v>14</v>
@@ -7703,7 +7703,7 @@
       </c>
       <c r="Z245">
         <f t="shared" si="114"/>
-        <v>9901746</v>
+        <v>9901534</v>
       </c>
       <c r="AB245" t="s">
         <v>15</v>
@@ -7734,7 +7734,7 @@
       </c>
       <c r="Z246">
         <f>Z245*Y245</f>
-        <v>257445396</v>
+        <v>257439884</v>
       </c>
       <c r="AB246" t="s">
         <v>16</v>
@@ -7765,7 +7765,7 @@
       </c>
       <c r="Z247">
         <f t="shared" ref="Z247:Z250" si="118">Z246</f>
-        <v>257445396</v>
+        <v>257439884</v>
       </c>
       <c r="AB247" t="s">
         <v>12</v>
@@ -7796,7 +7796,7 @@
       </c>
       <c r="Z248">
         <f t="shared" si="118"/>
-        <v>257445396</v>
+        <v>257439884</v>
       </c>
       <c r="AB248" t="s">
         <v>17</v>
@@ -7827,7 +7827,7 @@
       </c>
       <c r="Z249">
         <f t="shared" si="118"/>
-        <v>257445396</v>
+        <v>257439884</v>
       </c>
       <c r="AB249" t="s">
         <v>31</v>
@@ -7857,7 +7857,7 @@
       </c>
       <c r="Z250">
         <f t="shared" si="118"/>
-        <v>257445396</v>
+        <v>257439884</v>
       </c>
       <c r="AB250" t="s">
         <v>14</v>
@@ -7888,7 +7888,7 @@
       </c>
       <c r="Z251">
         <f>Z250+Y250</f>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="AB251" t="s">
         <v>19</v>
@@ -7919,7 +7919,7 @@
       </c>
       <c r="Z252" s="3">
         <f t="shared" ref="Z252:Z256" si="121">Z251</f>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
     </row>
     <row r="253" spans="21:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7940,7 +7940,7 @@
       </c>
       <c r="Z253">
         <f t="shared" si="121"/>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="AB253" t="s">
         <v>4</v>
@@ -7971,7 +7971,7 @@
       </c>
       <c r="Z254">
         <f t="shared" si="121"/>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="AB254" t="s">
         <v>5</v>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="X255">
         <f>X254+Z254</f>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="Y255">
         <f t="shared" si="120"/>
@@ -8002,7 +8002,7 @@
       </c>
       <c r="Z255">
         <f t="shared" si="121"/>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="AB255" t="s">
         <v>6</v>
@@ -8033,7 +8033,7 @@
       </c>
       <c r="Z256">
         <f t="shared" si="121"/>
-        <v>257445408</v>
+        <v>257439896</v>
       </c>
       <c r="AB256" t="s">
         <v>7</v>
@@ -8063,8 +8063,8 @@
         <v>12</v>
       </c>
       <c r="Z257">
-        <f>Z256/AD257</f>
-        <v>9901746.461538462</v>
+        <f>TRUNC(Z256/AD257,0)</f>
+        <v>9901534</v>
       </c>
       <c r="AB257" s="6" t="s">
         <v>27</v>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="Z258">
         <f t="shared" ref="Z258:Z264" si="124">Z257</f>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB258" t="s">
         <v>28</v>
@@ -8128,13 +8128,13 @@
       </c>
       <c r="Z259">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB259" t="s">
         <v>10</v>
       </c>
       <c r="AE259">
-        <f t="shared" ref="AE259:AE270" si="125">IF(AB259=AG259,1,0)</f>
+        <f t="shared" ref="AE259:AE267" si="125">IF(AB259=AG259,1,0)</f>
         <v>1</v>
       </c>
       <c r="AG259" t="s">
@@ -8159,7 +8159,7 @@
       </c>
       <c r="Z260">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB260" t="s">
         <v>11</v>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="Z261">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB261" t="s">
         <v>12</v>
@@ -8221,7 +8221,7 @@
       </c>
       <c r="Z262">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB262" t="s">
         <v>13</v>
@@ -8252,7 +8252,7 @@
       </c>
       <c r="Z263">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB263" t="s">
         <v>14</v>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="Z264">
         <f t="shared" si="124"/>
-        <v>9901746.461538462</v>
+        <v>9901534</v>
       </c>
       <c r="AB264" t="s">
         <v>15</v>
@@ -8314,7 +8314,7 @@
       </c>
       <c r="Z265">
         <f>Z264*Y264</f>
-        <v>257445408</v>
+        <v>257439884</v>
       </c>
       <c r="AB265" t="s">
         <v>16</v>
@@ -8345,7 +8345,7 @@
       </c>
       <c r="Z266">
         <f t="shared" ref="Z266:Z269" si="128">Z265</f>
-        <v>257445408</v>
+        <v>257439884</v>
       </c>
       <c r="AB266" t="s">
         <v>12</v>
@@ -8376,7 +8376,7 @@
       </c>
       <c r="Z267">
         <f t="shared" si="128"/>
-        <v>257445408</v>
+        <v>257439884</v>
       </c>
       <c r="AB267" t="s">
         <v>17</v>
@@ -8407,7 +8407,7 @@
       </c>
       <c r="Z268">
         <f t="shared" si="128"/>
-        <v>257445408</v>
+        <v>257439884</v>
       </c>
       <c r="AB268" t="s">
         <v>39</v>
@@ -8437,7 +8437,7 @@
       </c>
       <c r="Z269">
         <f t="shared" si="128"/>
-        <v>257445408</v>
+        <v>257439884</v>
       </c>
       <c r="AB269" t="s">
         <v>14</v>
@@ -8468,7 +8468,7 @@
       </c>
       <c r="Z270">
         <f>Z269+Y269</f>
-        <v>257445419</v>
+        <v>257439895</v>
       </c>
       <c r="AB270" t="s">
         <v>19</v>
@@ -8499,7 +8499,7 @@
       </c>
       <c r="Z271" s="3">
         <f t="shared" ref="Z271" si="131">Z270</f>
-        <v>257445419</v>
+        <v>257439895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>